<commit_message>
Update fonts in excel file
</commit_message>
<xml_diff>
--- a/docs/01-basics/pie-chart-overview.xlsx
+++ b/docs/01-basics/pie-chart-overview.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11013"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.kluesener\Desktop\Ablage\3-ITech\1-Schulungen\4-BLOCKCHAIN\isaqb-blockchain\docs\01-basics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/Documents/developer/github_isaqb/curriculum-blockchain/docs/01-basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5C38A24A-E125-B24F-A5DB-825DFA6DCA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6180" yWindow="1905" windowWidth="24555" windowHeight="17655" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4420" yWindow="460" windowWidth="24560" windowHeight="15540" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DE-Grafik" sheetId="3" r:id="rId1"/>
     <sheet name="EN-Graphic" sheetId="1" r:id="rId2"/>
     <sheet name="Tabelle1" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -32,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Vortrag</t>
   </si>
@@ -49,29 +53,37 @@
     <t>Smart Contracts</t>
   </si>
   <si>
+    <t>Blockchain flavours and their use cases</t>
+  </si>
+  <si>
     <t>Permissioned blockchain implementations</t>
   </si>
   <si>
     <t>Architecting Blockchain Applications</t>
   </si>
   <si>
-    <t>Blockchain flavours and their use cases</t>
+    <t>Example of Blockchain Architecture</t>
   </si>
   <si>
-    <t>Example of Blockchain Architecture</t>
+    <t>Beispiel einer Blockchain-Architektur</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -94,11 +106,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -114,9 +127,9 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -135,12 +148,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="4"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -149,8 +164,7 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -159,8 +173,7 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -169,8 +182,7 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -179,8 +191,7 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -189,8 +200,7 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
               </c:ext>
@@ -211,11 +221,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -232,57 +242,31 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="1.3940269456022822E-2"/>
-                  <c:y val="3.7075114655675243E-2"/>
+                  <c:x val="-3.0409101070568101E-2"/>
+                  <c:y val="6.7844132435252794E-2"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
-                  <a:noAutofit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.28426437220278761"/>
-                      <c:h val="0.14043870366332439"/>
-                    </c:manualLayout>
-                  </c15:layout>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -300,11 +284,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -321,11 +305,11 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
                 </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -342,10 +326,7 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                  <c16:uniqueId val="{00000005-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
-                </c:ext>
+              <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout>
                     <c:manualLayout>
@@ -353,6 +334,9 @@
                       <c:h val="0.19607003390775066"/>
                     </c:manualLayout>
                   </c15:layout>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -370,15 +354,15 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'DE-Grafik'!$A$1:$A$5</c:f>
+              <c:f>'DE-Grafik'!$A$1:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>Blockchain overview and basics</c:v>
                 </c:pt>
@@ -386,42 +370,48 @@
                   <c:v>Smart Contracts</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>Blockchain flavours and their use cases</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>Permissioned blockchain implementations</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>Architecting Blockchain Applications</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>Blockchain flavours and their use cases</c:v>
+                <c:pt idx="5">
+                  <c:v>Beispiel einer Blockchain-Architektur</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'DE-Grafik'!$B$1:$B$5</c:f>
+              <c:f>'DE-Grafik'!$B$1:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>300</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-A4C3-CF4A-A4D5-5E2A8878AA85}"/>
             </c:ext>
@@ -453,9 +443,12 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1800"/>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -467,9 +460,9 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -488,12 +481,14 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:explosion val="19"/>
+          <c:spPr>
+            <a:effectLst/>
+          </c:spPr>
+          <c:explosion val="4"/>
           <c:dPt>
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -502,8 +497,7 @@
           <c:dPt>
             <c:idx val="1"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="5"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -512,8 +506,7 @@
           <c:dPt>
             <c:idx val="2"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -522,8 +515,7 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="6"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -532,8 +524,7 @@
           <c:dPt>
             <c:idx val="4"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="8"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -542,8 +533,7 @@
           <c:dPt>
             <c:idx val="5"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="7"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-01D3-8347-BAD4-8610D9832016}"/>
               </c:ext>
@@ -564,12 +554,10 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000000-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -587,12 +575,10 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -600,46 +586,20 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.1750924749185499E-3"/>
-                  <c:y val="-1.0744612244793997E-16"/>
+                  <c:x val="0.19036064261784397"/>
+                  <c:y val="1.0430393951072285E-16"/>
                 </c:manualLayout>
               </c:layout>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
-                  <a:noAutofit/>
-                </a:bodyPr>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr/>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="1"/>
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000002-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout>
-                    <c:manualLayout>
-                      <c:w val="0.28909030343894948"/>
-                      <c:h val="0.15117844069032432"/>
-                    </c:manualLayout>
-                  </c15:layout>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -657,12 +617,10 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -670,8 +628,8 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.82861803157886E-2"/>
-                  <c:y val="-5.3475002371691498E-2"/>
+                  <c:x val="-5.8226699899333038E-2"/>
+                  <c:y val="-2.5028082872191854E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -680,12 +638,10 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -693,8 +649,8 @@
               <c:idx val="5"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="3.6632802603144602E-3"/>
-                  <c:y val="-3.2186462384972997E-2"/>
+                  <c:x val="-2.6959596829617984E-2"/>
+                  <c:y val="0"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -703,12 +659,17 @@
               <c:showSerName val="0"/>
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
-              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout>
+                    <c:manualLayout>
+                      <c:w val="0.24935591521722356"/>
+                      <c:h val="0.15194900172809059"/>
+                    </c:manualLayout>
+                  </c15:layout>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-01D3-8347-BAD4-8610D9832016}"/>
-                </c:ext>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -726,7 +687,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -783,7 +744,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000006-01D3-8347-BAD4-8610D9832016}"/>
             </c:ext>
@@ -815,9 +776,12 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr sz="1600"/>
+        <a:defRPr sz="1400">
+          <a:latin typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+          <a:ea typeface="Roboto" panose="02000000000000000000" pitchFamily="2" charset="0"/>
+        </a:defRPr>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -834,13 +798,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -848,7 +812,7 @@
         <xdr:cNvPr id="2" name="Diagramm 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -877,21 +841,21 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25399</xdr:rowOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>53411</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Diagramm 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1233,77 +1197,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
-        <v>300</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" s="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>180</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
         <v>120</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
         <v>240</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>240</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <f>SUM(B1:B5)</f>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
+        <f>SUM(B1:B6)</f>
         <v>1080</v>
       </c>
     </row>
@@ -1315,69 +1274,71 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="1" max="1" width="40.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="42" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>270</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="1">
         <f>SUM(B1:B6)</f>
         <v>1080</v>
       </c>
@@ -1389,130 +1350,133 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView zoomScale="249" zoomScaleNormal="249" zoomScalePageLayoutView="249" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>15</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <f>B2+C2</f>
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>120</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <f t="shared" ref="D3:D8" si="0">B3+C3</f>
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>300</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>90</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <f t="shared" si="0"/>
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>150</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>90</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>60</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>30</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>45</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>60</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="1">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D10">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="1">
         <f>SUM(D2:D8)</f>
         <v>960</v>
       </c>

</xml_diff>